<commit_message>
updated no degree data, added top degree list
</commit_message>
<xml_diff>
--- a/speakers.xlsx
+++ b/speakers.xlsx
@@ -13,10 +13,10 @@
   <definedNames/>
   <calcPr/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId9"/>
-    <pivotCache cacheId="0" r:id="rId10"/>
-    <pivotCache cacheId="4" r:id="rId11"/>
-    <pivotCache cacheId="3" r:id="rId12"/>
+    <pivotCache cacheId="3" r:id="rId9"/>
+    <pivotCache cacheId="4" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
     <pivotCache cacheId="2" r:id="rId13"/>
   </pivotCaches>
 </workbook>
@@ -79,7 +79,7 @@
     <t>~36</t>
   </si>
   <si>
-    <t>(no degree)</t>
+    <t>No Degree</t>
   </si>
   <si>
     <t>BALR</t>
@@ -3117,6 +3117,136 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E1:E336" sheet="Raw Data"/>
+  </cacheSource>
+  <cacheFields>
+    <cacheField name="degree from">
+      <sharedItems containsBlank="1">
+        <s v="University of California at Berkeley"/>
+        <s v="No Degree"/>
+        <s v="University of Illinois at Urbana-Champaign"/>
+        <s v="Stanford University"/>
+        <m/>
+        <s v="Cornell University"/>
+        <s v="Purdue University"/>
+        <s v="University of Bristol"/>
+        <s v="University of Wisconsin-Madison"/>
+        <s v="Massachusetts Institute of Technology"/>
+        <s v="Arizona State University"/>
+        <s v="University of Pennsylvania"/>
+        <s v="Cambridge University"/>
+        <s v="Rockford College"/>
+        <s v="Michigan State University"/>
+        <s v="University of California at Davis"/>
+        <s v="The Ohio State University"/>
+        <s v="University of California at Irvine"/>
+        <s v="Humboldt University"/>
+        <s v="Northwestern University"/>
+        <s v="University of Illinois Chicago"/>
+        <s v="Carnegie Mellon University"/>
+        <s v="University of Amsterdam"/>
+        <s v="University of Southern California"/>
+        <s v="University of Calgary"/>
+        <s v="Syracuse"/>
+        <s v="Foothill College"/>
+        <s v="Moscow Institute of Aviation"/>
+        <s v="University of Nevada at Las Vegas"/>
+        <s v="University of Maryland"/>
+        <s v="Lancaster University"/>
+        <s v="University of New South Wales"/>
+        <s v="Technical University of Denmark"/>
+        <s v="Princeton University"/>
+        <s v="University of Chicago"/>
+        <s v="Kyoto University"/>
+        <s v="University of California at Los Angeles"/>
+        <s v="Duke University"/>
+        <s v="University of Alabama"/>
+        <s v="University of Connecticut"/>
+        <s v="University of Missouri Columbia"/>
+        <s v="Portland State University"/>
+        <s v="University of Cincinnati"/>
+        <s v="Florida Atlantic University"/>
+        <s v="California Institute of Technology"/>
+        <s v="University of Lund"/>
+        <s v="Illinois Institute of Technology"/>
+        <s v="University of Vienna"/>
+        <s v="University of Michigan"/>
+        <s v="University of California at Santa Barbara"/>
+        <s v="Reed College"/>
+        <s v="Washington University Saint Louis"/>
+        <s v="Imperial College"/>
+        <s v="University of Texas at Austin"/>
+        <s v="Slade School of Fine Arts"/>
+        <s v="Harvard University"/>
+        <s v="Union College"/>
+        <s v="Yale University"/>
+        <s v="University of Washington"/>
+        <s v="Dalhousie"/>
+        <s v="Mississippi State University"/>
+        <s v="Indiana University"/>
+        <s v="North Dakota State University"/>
+        <s v="Brown University"/>
+        <s v="University of Delaware "/>
+        <s v="University of Western Ontario"/>
+        <s v="Johns Hopkins Univ"/>
+        <s v="Loyola University of Chicago"/>
+        <s v="Liceo Scientifico Copernico, Bologna"/>
+        <s v="Delft University of Technology"/>
+        <s v="University of Virginia"/>
+        <s v="Carleton University"/>
+        <s v="Tufts University"/>
+        <s v="Johns Hopkins University"/>
+        <s v="University of Iowa"/>
+        <s v="Rice University"/>
+        <s v="Drexel University"/>
+        <s v="University of Oregon"/>
+        <s v="Harvey Mudd College"/>
+        <s v="Piedmont Community College"/>
+        <s v="St. Mary's College of California"/>
+        <s v="Hampshire College"/>
+        <s v="University of Toronto"/>
+        <s v="Technische Universitaet Muenchen"/>
+        <s v="Case Western Reserve University"/>
+        <s v="University of Bologna"/>
+        <s v="University of Illinois"/>
+        <s v="College of Dublin"/>
+        <s v="Univerisity of Illinois"/>
+        <s v="DeVry University"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="D1:D336" sheet="Raw Data"/>
+  </cacheSource>
+  <cacheFields>
+    <cacheField name="degree">
+      <sharedItems containsBlank="1">
+        <s v="BS"/>
+        <s v="No Degree"/>
+        <s v="PhD"/>
+        <s v="MS"/>
+        <m/>
+        <s v="MFA"/>
+        <s v="Sc.D"/>
+        <s v="DA"/>
+        <s v="MBA"/>
+        <s v="MA"/>
+        <s v="BA"/>
+        <s v="AB"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
   <cacheSource type="worksheet">
     <worksheetSource ref="H1:J336" sheet="Raw Data"/>
@@ -3222,7 +3352,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
   <cacheSource type="worksheet">
     <worksheetSource ref="F1:F336" sheet="Raw Data"/>
@@ -3233,136 +3363,6 @@
         <s v="M"/>
         <m/>
         <s v="F"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="D1:D336" sheet="Raw Data"/>
-  </cacheSource>
-  <cacheFields>
-    <cacheField name="degree">
-      <sharedItems containsBlank="1">
-        <s v="BS"/>
-        <s v="(no degree)"/>
-        <s v="PhD"/>
-        <s v="MS"/>
-        <m/>
-        <s v="MFA"/>
-        <s v="Sc.D"/>
-        <s v="DA"/>
-        <s v="MBA"/>
-        <s v="MA"/>
-        <s v="BA"/>
-        <s v="AB"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="E1:E336" sheet="Raw Data"/>
-  </cacheSource>
-  <cacheFields>
-    <cacheField name="degree from">
-      <sharedItems containsBlank="1">
-        <s v="University of California at Berkeley"/>
-        <s v="(no degree)"/>
-        <s v="University of Illinois at Urbana-Champaign"/>
-        <s v="Stanford University"/>
-        <m/>
-        <s v="Cornell University"/>
-        <s v="Purdue University"/>
-        <s v="University of Bristol"/>
-        <s v="University of Wisconsin-Madison"/>
-        <s v="Massachusetts Institute of Technology"/>
-        <s v="Arizona State University"/>
-        <s v="University of Pennsylvania"/>
-        <s v="Cambridge University"/>
-        <s v="Rockford College"/>
-        <s v="Michigan State University"/>
-        <s v="University of California at Davis"/>
-        <s v="The Ohio State University"/>
-        <s v="University of California at Irvine"/>
-        <s v="Humboldt University"/>
-        <s v="Northwestern University"/>
-        <s v="University of Illinois Chicago"/>
-        <s v="Carnegie Mellon University"/>
-        <s v="University of Amsterdam"/>
-        <s v="University of Southern California"/>
-        <s v="University of Calgary"/>
-        <s v="Syracuse"/>
-        <s v="Foothill College"/>
-        <s v="Moscow Institute of Aviation"/>
-        <s v="University of Nevada at Las Vegas"/>
-        <s v="University of Maryland"/>
-        <s v="Lancaster University"/>
-        <s v="University of New South Wales"/>
-        <s v="Technical University of Denmark"/>
-        <s v="Princeton University"/>
-        <s v="University of Chicago"/>
-        <s v="Kyoto University"/>
-        <s v="University of California at Los Angeles"/>
-        <s v="Duke University"/>
-        <s v="University of Alabama"/>
-        <s v="University of Connecticut"/>
-        <s v="University of Missouri Columbia"/>
-        <s v="Portland State University"/>
-        <s v="University of Cincinnati"/>
-        <s v="Florida Atlantic University"/>
-        <s v="California Institute of Technology"/>
-        <s v="University of Lund"/>
-        <s v="Illinois Institute of Technology"/>
-        <s v="University of Vienna"/>
-        <s v="University of Michigan"/>
-        <s v="University of California at Santa Barbara"/>
-        <s v="Reed College"/>
-        <s v="Washington University Saint Louis"/>
-        <s v="Imperial College"/>
-        <s v="University of Texas at Austin"/>
-        <s v="Slade School of Fine Arts"/>
-        <s v="Harvard University"/>
-        <s v="Union College"/>
-        <s v="Yale University"/>
-        <s v="University of Washington"/>
-        <s v="Dalhousie"/>
-        <s v="Mississippi State University"/>
-        <s v="Indiana University"/>
-        <s v="North Dakota State University"/>
-        <s v="Brown University"/>
-        <s v="University of Delaware "/>
-        <s v="University of Western Ontario"/>
-        <s v="Johns Hopkins Univ"/>
-        <s v="Loyola University of Chicago"/>
-        <s v="Liceo Scientifico Copernico, Bologna"/>
-        <s v="Delft University of Technology"/>
-        <s v="University of Virginia"/>
-        <s v="Carleton University"/>
-        <s v="Tufts University"/>
-        <s v="Johns Hopkins University"/>
-        <s v="University of Iowa"/>
-        <s v="Rice University"/>
-        <s v="Drexel University"/>
-        <s v="University of Oregon"/>
-        <s v="Harvey Mudd College"/>
-        <s v="Piedmont Community College"/>
-        <s v="St. Mary's College of California"/>
-        <s v="Hampshire College"/>
-        <s v="University of Toronto"/>
-        <s v="Technische Universitaet Muenchen"/>
-        <s v="Case Western Reserve University"/>
-        <s v="University of Bologna"/>
-        <s v="University of Illinois"/>
-        <s v="College of Dublin"/>
-        <s v="Univerisity of Illinois"/>
-        <s v="DeVry University"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -3864,7 +3864,6 @@
     <pivotField axis="axisRow" name="degree from" sortType="ascending" showAll="0" dataField="1" outline="0" multipleItemSelectionAllowed="1">
       <items>
         <item x="4"/>
-        <item x="1"/>
         <item x="10"/>
         <item x="63"/>
         <item x="44"/>
@@ -3898,6 +3897,7 @@
         <item x="14"/>
         <item x="60"/>
         <item x="27"/>
+        <item x="1"/>
         <item x="62"/>
         <item x="19"/>
         <item x="79"/>
@@ -8679,13 +8679,13 @@
       <c t="s" s="2" r="B116">
         <v>313</v>
       </c>
-      <c t="s" s="2" r="C116">
-        <v>18</v>
-      </c>
+      <c s="2" r="C116"/>
       <c t="s" s="2" r="D116">
         <v>18</v>
       </c>
-      <c s="2" r="E116"/>
+      <c t="s" s="2" r="E116">
+        <v>18</v>
+      </c>
       <c t="s" s="2" r="F116">
         <v>15</v>
       </c>
@@ -8723,13 +8723,13 @@
       <c t="s" s="2" r="B117">
         <v>315</v>
       </c>
-      <c t="s" s="2" r="C117">
-        <v>18</v>
-      </c>
+      <c s="2" r="C117"/>
       <c t="s" s="2" r="D117">
         <v>18</v>
       </c>
-      <c s="2" r="E117"/>
+      <c t="s" s="2" r="E117">
+        <v>18</v>
+      </c>
       <c t="s" s="2" r="F117">
         <v>15</v>
       </c>
@@ -8767,13 +8767,13 @@
       <c t="s" s="2" r="B118">
         <v>316</v>
       </c>
-      <c t="s" s="2" r="C118">
-        <v>18</v>
-      </c>
+      <c s="2" r="C118"/>
       <c t="s" s="2" r="D118">
         <v>18</v>
       </c>
-      <c s="2" r="E118"/>
+      <c t="s" s="2" r="E118">
+        <v>18</v>
+      </c>
       <c t="s" s="2" r="F118">
         <v>15</v>
       </c>

</xml_diff>